<commit_message>
Added soft constraint for division fairness within each period
# - Introduced slack variables for division-period fairness
# - Incorporated new constraints to encourage proportional division assignments per period
# - Penalized deviations in the objective function with a lower weight to make this constraint less important than existing ones
</commit_message>
<xml_diff>
--- a/apps/files/ngs-fairness-solver-files-output/deployment_report.xlsx
+++ b/apps/files/ngs-fairness-solver-files-output/deployment_report.xlsx
@@ -7,18 +7,18 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SA_G1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="A_G1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="SA_G2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="A_G2" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="SA_G3" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="A_G3" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="SA_G4" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="A_G4" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="SA_S1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="A_S1" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="SA_S2" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="A_S2" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="SA_19.8 - 25.8" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="A_19.8 - 25.8" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SA_27.10 - 2.11" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="A_27.10 - 2.11" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SA_3.11 - 16.11" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="A_3.11 - 16.11" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SA_17.11 - 22.11" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="A_17.11 - 22.11" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="SA_2.9 - 8.9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="A_2.9 - 8.9" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="SA_30.11 - 15.12" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="A_30.11 - 15.12" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="Overall_Summary" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -525,7 +525,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -560,22 +560,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -588,13 +588,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -616,13 +616,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -635,22 +635,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -746,19 +746,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>2</v>
@@ -777,10 +777,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -802,13 +802,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>2</v>
@@ -824,19 +824,19 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -846,16 +846,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -938,13 +938,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
@@ -966,13 +966,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -988,16 +988,16 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -1007,13 +1007,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -1022,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1044,10 +1044,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -1057,22 +1057,22 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
         <v>4</v>
       </c>
-      <c r="D7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
       <c r="F7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1096,9 +1096,9 @@
   <cols>
     <col width="7" customWidth="1" min="1" max="1"/>
     <col width="3" customWidth="1" min="2" max="2"/>
-    <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="4" customWidth="1" min="3" max="3"/>
     <col width="3" customWidth="1" min="4" max="4"/>
-    <col width="4" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="5" max="5"/>
     <col width="3" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
   </cols>
@@ -1149,16 +1149,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -1177,13 +1177,13 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -1193,7 +1193,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
@@ -1202,13 +1202,13 @@
         <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -1221,19 +1221,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -1249,16 +1249,16 @@
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -1268,22 +1268,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>19.42%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20.39%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>20.39%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>20.39%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>19.42%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>16.50%</t>
+          <t>18.00%</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>21.36%</t>
+          <t>21.00%</t>
         </is>
       </c>
     </row>
@@ -1474,7 +1474,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>20.39%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>18.45%</t>
+          <t>18.00%</t>
         </is>
       </c>
     </row>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>23.30%</t>
+          <t>23.00%</t>
         </is>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>19.82%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>19.82%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>20.28%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>20.28%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>19.82%</t>
+          <t>20.00%</t>
         </is>
       </c>
     </row>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>17.51%</t>
+          <t>17.50%</t>
         </is>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>21.20%</t>
+          <t>22.00%</t>
         </is>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>20.74%</t>
+          <t>20.50%</t>
         </is>
       </c>
     </row>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17.97%</t>
+          <t>17.50%</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>22.58%</t>
+          <t>22.50%</t>
         </is>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -1790,7 +1790,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1815,10 +1815,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1830,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1840,10 +1840,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1868,19 +1868,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
         <v>3</v>
@@ -1899,13 +1899,13 @@
         <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1976,10 +1976,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2004,10 +2004,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -2016,7 +2016,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -2026,7 +2026,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -2035,13 +2035,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -2051,22 +2051,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -2082,13 +2082,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>4</v>
@@ -2101,22 +2101,22 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" t="n">
         <v>3</v>
       </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>4</v>
-      </c>
       <c r="G7" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2187,22 +2187,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -2212,22 +2212,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -2237,13 +2237,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
@@ -2252,7 +2252,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -2265,19 +2265,19 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -2287,22 +2287,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -2312,19 +2312,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G7" t="n">
         <v>30</v>
@@ -2352,7 +2352,7 @@
     <col width="7" customWidth="1" min="1" max="1"/>
     <col width="3" customWidth="1" min="2" max="2"/>
     <col width="3" customWidth="1" min="3" max="3"/>
-    <col width="3" customWidth="1" min="4" max="4"/>
+    <col width="4" customWidth="1" min="4" max="4"/>
     <col width="3" customWidth="1" min="5" max="5"/>
     <col width="3" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
@@ -2398,22 +2398,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -2423,22 +2423,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -2457,13 +2457,13 @@
         <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -2476,7 +2476,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>2</v>
@@ -2485,10 +2485,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -2498,13 +2498,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
@@ -2523,19 +2523,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
         <v>9</v>
       </c>
       <c r="D7" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E7" t="n">
         <v>8</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
         <v>40</v>
@@ -2609,22 +2609,22 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
       </c>
       <c r="F2" t="n">
         <v>4</v>
       </c>
       <c r="G2" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -2634,10 +2634,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>4</v>
@@ -2649,7 +2649,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -2668,13 +2668,13 @@
         <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -2687,19 +2687,19 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -2709,7 +2709,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
         <v>4</v>
@@ -2721,7 +2721,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G6" t="n">
         <v>18</v>
@@ -2734,22 +2734,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
         <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G7" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2820,7 +2820,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -2835,7 +2835,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -2848,19 +2848,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -2870,22 +2870,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -2895,10 +2895,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -2907,10 +2907,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -2926,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -2935,7 +2935,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -2945,22 +2945,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G7" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3031,22 +3031,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -3056,7 +3056,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -3071,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -3087,16 +3087,16 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -3106,22 +3106,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -3137,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
@@ -3146,7 +3146,7 @@
         <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -3156,22 +3156,22 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" t="n">
         <v>8</v>
       </c>
-      <c r="C7" t="n">
+      <c r="F7" t="n">
         <v>8</v>
       </c>
-      <c r="D7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6</v>
-      </c>
       <c r="G7" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3248,13 +3248,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -3267,22 +3267,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -3298,7 +3298,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -3329,10 +3329,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -3354,10 +3354,10 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -3367,22 +3367,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Break tol into div and watch tol
</commit_message>
<xml_diff>
--- a/apps/files/ngs-fairness-solver-files-output/deployment_report.xlsx
+++ b/apps/files/ngs-fairness-solver-files-output/deployment_report.xlsx
@@ -7,19 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SA_19.8 - 25.8" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="A_19.8 - 25.8" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="SA_27.10 - 2.11" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="A_27.10 - 2.11" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="SA_3.11 - 16.11" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="A_3.11 - 16.11" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="SA_17.11 - 22.11" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="A_17.11 - 22.11" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="SA_2.9 - 8.9" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="A_2.9 - 8.9" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="SA_30.11 - 15.12" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="A_30.11 - 15.12" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Overall_Summary" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="SA_NG1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="A_NG1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SA_NG2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="A_NG2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SA_NG4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="A_NG4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SA_NGD1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="A_NGD1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Overall_Summary" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -513,13 +509,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -566,13 +562,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
@@ -613,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -622,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>1</v>
@@ -641,1060 +637,16 @@
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
-    <col width="3" customWidth="1" min="2" max="2"/>
-    <col width="3" customWidth="1" min="3" max="3"/>
-    <col width="3" customWidth="1" min="4" max="4"/>
-    <col width="3" customWidth="1" min="5" max="5"/>
-    <col width="3" customWidth="1" min="6" max="6"/>
-    <col width="7" customWidth="1" min="7" max="7"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="n"/>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>HOS</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>KWL</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>KCE</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>NTE</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>NTW</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
-    <col width="3" customWidth="1" min="2" max="2"/>
-    <col width="3" customWidth="1" min="3" max="3"/>
-    <col width="3" customWidth="1" min="4" max="4"/>
-    <col width="3" customWidth="1" min="5" max="5"/>
-    <col width="3" customWidth="1" min="6" max="6"/>
-    <col width="7" customWidth="1" min="7" max="7"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="n"/>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>HOS</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>KWL</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>KCE</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>NTE</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>NTW</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" t="n">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
-    <col width="3" customWidth="1" min="2" max="2"/>
-    <col width="4" customWidth="1" min="3" max="3"/>
-    <col width="3" customWidth="1" min="4" max="4"/>
-    <col width="3" customWidth="1" min="5" max="5"/>
-    <col width="3" customWidth="1" min="6" max="6"/>
-    <col width="7" customWidth="1" min="7" max="7"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="n"/>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>HOS</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>KWL</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>KCE</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>NTE</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>NTW</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" t="n">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Rank</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Total Deployments</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Watch Actual - A</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Watch Actual - B</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Watch Actual - C</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Watch Actual - D</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Watch Actual - E</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Division Actual - HOS</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>18.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Division Actual - KCE</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>21.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Division Actual - KWL</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Division Actual - NTE</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>18.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>SA</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Division Actual - NTW</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>23.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Total Deployments</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Watch Actual - A</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Watch Actual - B</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Watch Actual - C</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Watch Actual - D</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Watch Actual - E</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>20.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Division Actual - HOS</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>17.50%</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Division Actual - KCE</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>22.00%</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Division Actual - KWL</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>20.50%</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Division Actual - NTE</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>17.50%</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Division Actual - NTW</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>22.50%</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -1771,10 +723,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -1793,16 +745,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>2</v>
@@ -1818,16 +770,16 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>2</v>
@@ -1843,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1852,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>2</v>
@@ -1868,10 +820,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1899,10 +851,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
         <v>10</v>
@@ -1976,13 +928,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -2007,7 +959,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -2016,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -2029,19 +981,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -2051,22 +1003,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -2104,13 +1056,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
@@ -2199,10 +1151,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -2215,19 +1167,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -2243,13 +1195,13 @@
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
         <v>7</v>
@@ -2271,13 +1223,13 @@
         <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -2287,7 +1239,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -2296,7 +1248,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
@@ -2312,19 +1264,19 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
         <v>7</v>
       </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6</v>
-      </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G7" t="n">
         <v>30</v>
@@ -2352,7 +1304,7 @@
     <col width="7" customWidth="1" min="1" max="1"/>
     <col width="3" customWidth="1" min="2" max="2"/>
     <col width="3" customWidth="1" min="3" max="3"/>
-    <col width="4" customWidth="1" min="4" max="4"/>
+    <col width="3" customWidth="1" min="4" max="4"/>
     <col width="3" customWidth="1" min="5" max="5"/>
     <col width="3" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
@@ -2398,13 +1350,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
@@ -2413,7 +1365,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -2423,22 +1375,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -2448,22 +1400,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -2473,22 +1425,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -2501,19 +1453,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -2523,22 +1475,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F7" t="n">
         <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2561,11 +1513,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="7" customWidth="1" min="1" max="1"/>
-    <col width="4" customWidth="1" min="2" max="2"/>
-    <col width="4" customWidth="1" min="3" max="3"/>
-    <col width="4" customWidth="1" min="4" max="4"/>
-    <col width="4" customWidth="1" min="5" max="5"/>
-    <col width="4" customWidth="1" min="6" max="6"/>
+    <col width="3" customWidth="1" min="2" max="2"/>
+    <col width="3" customWidth="1" min="3" max="3"/>
+    <col width="3" customWidth="1" min="4" max="4"/>
+    <col width="3" customWidth="1" min="5" max="5"/>
+    <col width="3" customWidth="1" min="6" max="6"/>
     <col width="7" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2609,22 +1561,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -2634,22 +1586,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -2659,22 +1611,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -2684,22 +1636,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -2712,19 +1664,19 @@
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -2734,22 +1686,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F7" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G7" t="n">
-        <v>80</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2823,19 +1775,19 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -2851,16 +1803,16 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -2870,22 +1822,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -2901,16 +1853,16 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -2920,22 +1872,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -2945,22 +1897,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3031,22 +1983,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -3056,22 +2008,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -3081,22 +2033,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -3106,22 +2058,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -3131,22 +2083,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -3156,22 +2108,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3185,7 +2137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3193,196 +2145,396 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
-    <col width="3" customWidth="1" min="2" max="2"/>
-    <col width="3" customWidth="1" min="3" max="3"/>
-    <col width="3" customWidth="1" min="4" max="4"/>
-    <col width="3" customWidth="1" min="5" max="5"/>
-    <col width="3" customWidth="1" min="6" max="6"/>
-    <col width="7" customWidth="1" min="7" max="7"/>
+    <col width="6" customWidth="1" min="1" max="1"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="n"/>
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
       <c r="B1" s="3" t="inlineStr">
         <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Total Deployments</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Watch Actual - A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Watch Actual - B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Watch Actual - C</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Watch Actual - D</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Watch Actual - E</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>18.18%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Division Actual - HOS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>15.91%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Division Actual - KCE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>22.73%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Division Actual - KWL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>22.73%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Division Actual - NTE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>15.91%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Division Actual - NTW</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>22.73%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>HOS</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>KWL</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>KCE</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>NTE</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="inlineStr">
-        <is>
-          <t>NTW</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" t="n">
-        <v>5</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Total Deployments</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Watch Actual - A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Watch Actual - B</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>19.32%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Watch Actual - C</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Watch Actual - D</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>19.32%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Watch Actual - E</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Division Actual - HOS</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>17.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Division Actual - KCE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>22.73%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Division Actual - KWL</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Division Actual - NTE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>17.05%</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Division Actual - NTW</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>22.73%</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>